<commit_message>
adding surrounding text to rmd analysis doc
</commit_message>
<xml_diff>
--- a/data/design.xlsx
+++ b/data/design.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nawis/GitHub/MicroMarsh/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E1565F9F-8C0D-5A47-A960-55AFAF6440E9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D995A1-B1AC-5D4D-BA90-02218E28F7A9}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1460" windowWidth="23960" windowHeight="14000" xr2:uid="{92964054-0BFF-F740-ADA1-1FABD046F48B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="152">
   <si>
     <t>sample_ID</t>
   </si>
@@ -301,6 +301,186 @@
   </si>
   <si>
     <t>03_14_PU5</t>
+  </si>
+  <si>
+    <t>07_15_C2</t>
+  </si>
+  <si>
+    <t>07_15_C1</t>
+  </si>
+  <si>
+    <t>10_15_C1</t>
+  </si>
+  <si>
+    <t>10_15_C2</t>
+  </si>
+  <si>
+    <t>10_16_C1</t>
+  </si>
+  <si>
+    <t>10_16_C2</t>
+  </si>
+  <si>
+    <t>07_17_C1</t>
+  </si>
+  <si>
+    <t>07_17_C2</t>
+  </si>
+  <si>
+    <t>07_15_CS2</t>
+  </si>
+  <si>
+    <t>07_15_CS3</t>
+  </si>
+  <si>
+    <t>10_15_CS2</t>
+  </si>
+  <si>
+    <t>10_15_CS3</t>
+  </si>
+  <si>
+    <t>10_16_CS2</t>
+  </si>
+  <si>
+    <t>10_16_CS3</t>
+  </si>
+  <si>
+    <t>07_15_F1</t>
+  </si>
+  <si>
+    <t>07_15_F2</t>
+  </si>
+  <si>
+    <t>10_15_F1</t>
+  </si>
+  <si>
+    <t>10_15_F2</t>
+  </si>
+  <si>
+    <t>10_16_F</t>
+  </si>
+  <si>
+    <t>10_16_F2</t>
+  </si>
+  <si>
+    <t>07_17_F1</t>
+  </si>
+  <si>
+    <t>07_17_F2</t>
+  </si>
+  <si>
+    <t>07_17_F6</t>
+  </si>
+  <si>
+    <t>07_15_PR1</t>
+  </si>
+  <si>
+    <t>07_15_PR2</t>
+  </si>
+  <si>
+    <t>10_15_PR1</t>
+  </si>
+  <si>
+    <t>10_15_PR2</t>
+  </si>
+  <si>
+    <t>10_16_PR1</t>
+  </si>
+  <si>
+    <t>10_16_PR2</t>
+  </si>
+  <si>
+    <t>07_17_PR1</t>
+  </si>
+  <si>
+    <t>07_17_PR2</t>
+  </si>
+  <si>
+    <t>07_17_PR3</t>
+  </si>
+  <si>
+    <t>07_17_PR4</t>
+  </si>
+  <si>
+    <t>07_17_PR6</t>
+  </si>
+  <si>
+    <t>07_15_PU1</t>
+  </si>
+  <si>
+    <t>07_15_PU2</t>
+  </si>
+  <si>
+    <t>10_15_PU1</t>
+  </si>
+  <si>
+    <t>10_15_PU2</t>
+  </si>
+  <si>
+    <t>10_16_PU1</t>
+  </si>
+  <si>
+    <t>10_16_PU2</t>
+  </si>
+  <si>
+    <t>03_14_C2</t>
+  </si>
+  <si>
+    <t>03_14_C3</t>
+  </si>
+  <si>
+    <t>03_14_C4</t>
+  </si>
+  <si>
+    <t>03_14_C5</t>
+  </si>
+  <si>
+    <t>03_14_C6</t>
+  </si>
+  <si>
+    <t>03_14_CS2</t>
+  </si>
+  <si>
+    <t>03_14_CS4</t>
+  </si>
+  <si>
+    <t>03_14_CS5</t>
+  </si>
+  <si>
+    <t>03_14_CS6</t>
+  </si>
+  <si>
+    <t>03_14_F2</t>
+  </si>
+  <si>
+    <t>03_14_F3</t>
+  </si>
+  <si>
+    <t>03_14_F4</t>
+  </si>
+  <si>
+    <t>03_14_F6</t>
+  </si>
+  <si>
+    <t>03_14_PR1</t>
+  </si>
+  <si>
+    <t>03_14_PR2</t>
+  </si>
+  <si>
+    <t>03_14_PR4</t>
+  </si>
+  <si>
+    <t>03_14_PR6</t>
+  </si>
+  <si>
+    <t>03_14_PU2</t>
+  </si>
+  <si>
+    <t>03_14_PU4</t>
+  </si>
+  <si>
+    <t>03_14_PU6</t>
   </si>
 </sst>
 </file>
@@ -652,9 +832,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA1714B5-51D6-344F-872E-758BD17049A7}">
-  <dimension ref="A1:D79"/>
+  <dimension ref="A1:D139"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A116" workbookViewId="0">
+      <selection activeCell="A139" sqref="A139"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
@@ -674,7 +856,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>93</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
@@ -683,12 +865,12 @@
         <v>25</v>
       </c>
       <c r="D2">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>92</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
@@ -697,12 +879,12 @@
         <v>25</v>
       </c>
       <c r="D3">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
@@ -711,12 +893,12 @@
         <v>25</v>
       </c>
       <c r="D4">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
         <v>18</v>
@@ -725,40 +907,40 @@
         <v>25</v>
       </c>
       <c r="D5">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
         <v>25</v>
       </c>
       <c r="D6">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
         <v>25</v>
       </c>
       <c r="D7">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>3</v>
+        <v>94</v>
       </c>
       <c r="B8" t="s">
         <v>19</v>
@@ -767,12 +949,12 @@
         <v>25</v>
       </c>
       <c r="D8">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>95</v>
       </c>
       <c r="B9" t="s">
         <v>19</v>
@@ -781,15 +963,15 @@
         <v>25</v>
       </c>
       <c r="D9">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
         <v>25</v>
@@ -800,10 +982,10 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
         <v>25</v>
@@ -814,10 +996,10 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C12" t="s">
         <v>25</v>
@@ -828,10 +1010,10 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" t="s">
         <v>25</v>
@@ -842,139 +1024,139 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>96</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14" t="s">
         <v>25</v>
       </c>
       <c r="D14">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>97</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C15" t="s">
         <v>25</v>
       </c>
       <c r="D15">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C16" t="s">
         <v>25</v>
       </c>
       <c r="D16">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C17" t="s">
         <v>25</v>
       </c>
       <c r="D17">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>49</v>
+        <v>8</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D19">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>50</v>
+        <v>98</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D20">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>51</v>
+        <v>99</v>
       </c>
       <c r="B21" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D21">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B22" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B23" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D23">
         <v>4</v>
@@ -982,13 +1164,13 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B24" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D24">
         <v>5</v>
@@ -996,13 +1178,13 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B25" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D25">
         <v>6</v>
@@ -1010,10 +1192,10 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B26" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C26" t="s">
         <v>26</v>
@@ -1024,111 +1206,111 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>57</v>
+        <v>100</v>
       </c>
       <c r="B27" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C27" t="s">
         <v>26</v>
       </c>
       <c r="D27">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>58</v>
+        <v>101</v>
       </c>
       <c r="B28" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C28" t="s">
         <v>26</v>
       </c>
       <c r="D28">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="B29" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C29" t="s">
         <v>26</v>
       </c>
       <c r="D29">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="B30" t="s">
         <v>18</v>
       </c>
       <c r="C30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D30">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="B31" t="s">
         <v>18</v>
       </c>
       <c r="C31" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D31">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="B32" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D32">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>37</v>
+        <v>102</v>
       </c>
       <c r="B33" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C33" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D33">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>9</v>
+        <v>103</v>
       </c>
       <c r="B34" t="s">
         <v>19</v>
       </c>
       <c r="C34" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D34">
         <v>3</v>
@@ -1136,13 +1318,13 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
       <c r="B35" t="s">
         <v>19</v>
       </c>
       <c r="C35" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D35">
         <v>4</v>
@@ -1150,13 +1332,13 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>11</v>
+        <v>54</v>
       </c>
       <c r="B36" t="s">
         <v>19</v>
       </c>
       <c r="C36" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D36">
         <v>5</v>
@@ -1164,13 +1346,13 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>12</v>
+        <v>55</v>
       </c>
       <c r="B37" t="s">
         <v>19</v>
       </c>
       <c r="C37" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D37">
         <v>6</v>
@@ -1178,293 +1360,293 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>13</v>
+        <v>56</v>
       </c>
       <c r="B38" t="s">
         <v>20</v>
       </c>
       <c r="C38" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D38">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>14</v>
+        <v>104</v>
       </c>
       <c r="B39" t="s">
         <v>20</v>
       </c>
       <c r="C39" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D39">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>15</v>
+        <v>105</v>
       </c>
       <c r="B40" t="s">
         <v>20</v>
       </c>
       <c r="C40" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D40">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>16</v>
+        <v>57</v>
       </c>
       <c r="B41" t="s">
         <v>20</v>
       </c>
       <c r="C41" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D41">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="B42" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C42" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D42">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="B43" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C43" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D43">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>41</v>
+        <v>106</v>
       </c>
       <c r="B44" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C44" t="s">
         <v>27</v>
       </c>
       <c r="D44">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>60</v>
+        <v>107</v>
       </c>
       <c r="B45" t="s">
         <v>18</v>
       </c>
       <c r="C45" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D45">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>61</v>
+        <v>34</v>
       </c>
       <c r="B46" t="s">
         <v>18</v>
       </c>
       <c r="C46" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D46">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>62</v>
+        <v>35</v>
       </c>
       <c r="B47" t="s">
         <v>18</v>
       </c>
       <c r="C47" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D47">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>63</v>
+        <v>36</v>
       </c>
       <c r="B48" t="s">
         <v>18</v>
       </c>
       <c r="C48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D48">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>64</v>
+        <v>37</v>
       </c>
       <c r="B49" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C49" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D49">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>65</v>
+        <v>108</v>
       </c>
       <c r="B50" t="s">
         <v>19</v>
       </c>
       <c r="C50" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D50">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>66</v>
+        <v>109</v>
       </c>
       <c r="B51" t="s">
         <v>19</v>
       </c>
       <c r="C51" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D51">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>67</v>
+        <v>9</v>
       </c>
       <c r="B52" t="s">
         <v>19</v>
       </c>
       <c r="C52" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D52">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>68</v>
+        <v>10</v>
       </c>
       <c r="B53" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C53" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D53">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>69</v>
+        <v>11</v>
       </c>
       <c r="B54" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C54" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D54">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>70</v>
+        <v>12</v>
       </c>
       <c r="B55" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C55" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D55">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>71</v>
+        <v>110</v>
       </c>
       <c r="B56" t="s">
         <v>20</v>
       </c>
       <c r="C56" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D56">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>72</v>
+        <v>111</v>
       </c>
       <c r="B57" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C57" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D57">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>73</v>
+        <v>13</v>
       </c>
       <c r="B58" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C58" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D58">
         <v>3</v>
@@ -1472,13 +1654,13 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>74</v>
+        <v>14</v>
       </c>
       <c r="B59" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C59" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D59">
         <v>4</v>
@@ -1486,13 +1668,13 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>75</v>
+        <v>15</v>
       </c>
       <c r="B60" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C60" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D60">
         <v>5</v>
@@ -1500,13 +1682,13 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
-        <v>76</v>
+        <v>16</v>
       </c>
       <c r="B61" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C61" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D61">
         <v>6</v>
@@ -1514,254 +1696,1094 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" t="s">
-        <v>77</v>
+        <v>112</v>
       </c>
       <c r="B62" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C62" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D62">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" t="s">
-        <v>78</v>
+        <v>113</v>
       </c>
       <c r="B63" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C63" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D63">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" t="s">
-        <v>79</v>
+        <v>43</v>
       </c>
       <c r="B64" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C64" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D64">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" t="s">
-        <v>80</v>
+        <v>42</v>
       </c>
       <c r="B65" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C65" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D65">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" t="s">
-        <v>81</v>
+        <v>41</v>
       </c>
       <c r="B66" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C66" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D66">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" t="s">
-        <v>82</v>
+        <v>114</v>
       </c>
       <c r="B67" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C67" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D67">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" t="s">
-        <v>83</v>
+        <v>115</v>
       </c>
       <c r="B68" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C68" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D68">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" t="s">
-        <v>84</v>
+        <v>116</v>
       </c>
       <c r="B69" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C69" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D69">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70" t="s">
-        <v>38</v>
+        <v>60</v>
       </c>
       <c r="B70" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C70" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D70">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="71" spans="1:4">
       <c r="A71" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="B71" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C71" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D71">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" t="s">
-        <v>86</v>
+        <v>62</v>
       </c>
       <c r="B72" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C72" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D72">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="73" spans="1:4">
       <c r="A73" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="B73" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C73" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D73">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="74" spans="1:4">
       <c r="A74" t="s">
-        <v>40</v>
+        <v>117</v>
       </c>
       <c r="B74" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C74" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D74">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:4">
       <c r="A75" t="s">
-        <v>87</v>
+        <v>118</v>
       </c>
       <c r="B75" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C75" t="s">
         <v>28</v>
       </c>
       <c r="D75">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="B76" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C76" t="s">
         <v>28</v>
       </c>
       <c r="D76">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="B77" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C77" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D77">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="78" spans="1:4">
       <c r="A78" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="B78" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C78" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D78">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="79" spans="1:4">
       <c r="A79" t="s">
+        <v>67</v>
+      </c>
+      <c r="B79" t="s">
+        <v>19</v>
+      </c>
+      <c r="C79" t="s">
+        <v>28</v>
+      </c>
+      <c r="D79">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" t="s">
+        <v>119</v>
+      </c>
+      <c r="B80" t="s">
+        <v>20</v>
+      </c>
+      <c r="C80" t="s">
+        <v>28</v>
+      </c>
+      <c r="D80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" t="s">
+        <v>120</v>
+      </c>
+      <c r="B81" t="s">
+        <v>20</v>
+      </c>
+      <c r="C81" t="s">
+        <v>28</v>
+      </c>
+      <c r="D81">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82" t="s">
+        <v>68</v>
+      </c>
+      <c r="B82" t="s">
+        <v>20</v>
+      </c>
+      <c r="C82" t="s">
+        <v>28</v>
+      </c>
+      <c r="D82">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83" t="s">
+        <v>69</v>
+      </c>
+      <c r="B83" t="s">
+        <v>20</v>
+      </c>
+      <c r="C83" t="s">
+        <v>28</v>
+      </c>
+      <c r="D83">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84" t="s">
+        <v>70</v>
+      </c>
+      <c r="B84" t="s">
+        <v>20</v>
+      </c>
+      <c r="C84" t="s">
+        <v>28</v>
+      </c>
+      <c r="D84">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85" t="s">
+        <v>71</v>
+      </c>
+      <c r="B85" t="s">
+        <v>20</v>
+      </c>
+      <c r="C85" t="s">
+        <v>28</v>
+      </c>
+      <c r="D85">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="A86" t="s">
+        <v>121</v>
+      </c>
+      <c r="B86" t="s">
+        <v>21</v>
+      </c>
+      <c r="C86" t="s">
+        <v>28</v>
+      </c>
+      <c r="D86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
+      <c r="A87" t="s">
+        <v>122</v>
+      </c>
+      <c r="B87" t="s">
+        <v>21</v>
+      </c>
+      <c r="C87" t="s">
+        <v>28</v>
+      </c>
+      <c r="D87">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
+      <c r="A88" t="s">
+        <v>123</v>
+      </c>
+      <c r="B88" t="s">
+        <v>21</v>
+      </c>
+      <c r="C88" t="s">
+        <v>28</v>
+      </c>
+      <c r="D88">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
+      <c r="A89" t="s">
+        <v>124</v>
+      </c>
+      <c r="B89" t="s">
+        <v>21</v>
+      </c>
+      <c r="C89" t="s">
+        <v>28</v>
+      </c>
+      <c r="D89">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="A90" t="s">
+        <v>72</v>
+      </c>
+      <c r="B90" t="s">
+        <v>21</v>
+      </c>
+      <c r="C90" t="s">
+        <v>28</v>
+      </c>
+      <c r="D90">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91" t="s">
+        <v>125</v>
+      </c>
+      <c r="B91" t="s">
+        <v>21</v>
+      </c>
+      <c r="C91" t="s">
+        <v>28</v>
+      </c>
+      <c r="D91">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
+      <c r="A92" t="s">
+        <v>126</v>
+      </c>
+      <c r="B92" t="s">
+        <v>18</v>
+      </c>
+      <c r="C92" t="s">
+        <v>29</v>
+      </c>
+      <c r="D92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
+      <c r="A93" t="s">
+        <v>127</v>
+      </c>
+      <c r="B93" t="s">
+        <v>18</v>
+      </c>
+      <c r="C93" t="s">
+        <v>29</v>
+      </c>
+      <c r="D93">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
+      <c r="A94" t="s">
+        <v>73</v>
+      </c>
+      <c r="B94" t="s">
+        <v>18</v>
+      </c>
+      <c r="C94" t="s">
+        <v>29</v>
+      </c>
+      <c r="D94">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
+      <c r="A95" t="s">
+        <v>74</v>
+      </c>
+      <c r="B95" t="s">
+        <v>18</v>
+      </c>
+      <c r="C95" t="s">
+        <v>29</v>
+      </c>
+      <c r="D95">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
+      <c r="A96" t="s">
+        <v>75</v>
+      </c>
+      <c r="B96" t="s">
+        <v>18</v>
+      </c>
+      <c r="C96" t="s">
+        <v>29</v>
+      </c>
+      <c r="D96">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
+      <c r="A97" t="s">
+        <v>76</v>
+      </c>
+      <c r="B97" t="s">
+        <v>18</v>
+      </c>
+      <c r="C97" t="s">
+        <v>29</v>
+      </c>
+      <c r="D97">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
+      <c r="A98" t="s">
+        <v>128</v>
+      </c>
+      <c r="B98" t="s">
+        <v>19</v>
+      </c>
+      <c r="C98" t="s">
+        <v>29</v>
+      </c>
+      <c r="D98">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
+      <c r="A99" t="s">
+        <v>129</v>
+      </c>
+      <c r="B99" t="s">
+        <v>19</v>
+      </c>
+      <c r="C99" t="s">
+        <v>29</v>
+      </c>
+      <c r="D99">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
+      <c r="A100" t="s">
+        <v>77</v>
+      </c>
+      <c r="B100" t="s">
+        <v>19</v>
+      </c>
+      <c r="C100" t="s">
+        <v>29</v>
+      </c>
+      <c r="D100">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
+      <c r="A101" t="s">
+        <v>78</v>
+      </c>
+      <c r="B101" t="s">
+        <v>19</v>
+      </c>
+      <c r="C101" t="s">
+        <v>29</v>
+      </c>
+      <c r="D101">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
+      <c r="A102" t="s">
+        <v>79</v>
+      </c>
+      <c r="B102" t="s">
+        <v>19</v>
+      </c>
+      <c r="C102" t="s">
+        <v>29</v>
+      </c>
+      <c r="D102">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
+      <c r="A103" t="s">
+        <v>80</v>
+      </c>
+      <c r="B103" t="s">
+        <v>19</v>
+      </c>
+      <c r="C103" t="s">
+        <v>29</v>
+      </c>
+      <c r="D103">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4">
+      <c r="A104" t="s">
+        <v>130</v>
+      </c>
+      <c r="B104" t="s">
+        <v>20</v>
+      </c>
+      <c r="C104" t="s">
+        <v>29</v>
+      </c>
+      <c r="D104">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4">
+      <c r="A105" t="s">
+        <v>131</v>
+      </c>
+      <c r="B105" t="s">
+        <v>20</v>
+      </c>
+      <c r="C105" t="s">
+        <v>29</v>
+      </c>
+      <c r="D105">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4">
+      <c r="A106" t="s">
+        <v>81</v>
+      </c>
+      <c r="B106" t="s">
+        <v>20</v>
+      </c>
+      <c r="C106" t="s">
+        <v>29</v>
+      </c>
+      <c r="D106">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4">
+      <c r="A107" t="s">
+        <v>82</v>
+      </c>
+      <c r="B107" t="s">
+        <v>20</v>
+      </c>
+      <c r="C107" t="s">
+        <v>29</v>
+      </c>
+      <c r="D107">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4">
+      <c r="A108" t="s">
+        <v>83</v>
+      </c>
+      <c r="B108" t="s">
+        <v>20</v>
+      </c>
+      <c r="C108" t="s">
+        <v>29</v>
+      </c>
+      <c r="D108">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4">
+      <c r="A109" t="s">
+        <v>84</v>
+      </c>
+      <c r="B109" t="s">
+        <v>20</v>
+      </c>
+      <c r="C109" t="s">
+        <v>29</v>
+      </c>
+      <c r="D109">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4">
+      <c r="A110" t="s">
+        <v>38</v>
+      </c>
+      <c r="B110" t="s">
+        <v>22</v>
+      </c>
+      <c r="C110" t="s">
+        <v>25</v>
+      </c>
+      <c r="D110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4">
+      <c r="A111" t="s">
+        <v>132</v>
+      </c>
+      <c r="B111" t="s">
+        <v>22</v>
+      </c>
+      <c r="C111" t="s">
+        <v>25</v>
+      </c>
+      <c r="D111">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4">
+      <c r="A112" t="s">
+        <v>133</v>
+      </c>
+      <c r="B112" t="s">
+        <v>22</v>
+      </c>
+      <c r="C112" t="s">
+        <v>25</v>
+      </c>
+      <c r="D112">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4">
+      <c r="A113" t="s">
+        <v>134</v>
+      </c>
+      <c r="B113" t="s">
+        <v>22</v>
+      </c>
+      <c r="C113" t="s">
+        <v>25</v>
+      </c>
+      <c r="D113">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4">
+      <c r="A114" t="s">
+        <v>135</v>
+      </c>
+      <c r="B114" t="s">
+        <v>22</v>
+      </c>
+      <c r="C114" t="s">
+        <v>25</v>
+      </c>
+      <c r="D114">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4">
+      <c r="A115" t="s">
+        <v>136</v>
+      </c>
+      <c r="B115" t="s">
+        <v>22</v>
+      </c>
+      <c r="C115" t="s">
+        <v>25</v>
+      </c>
+      <c r="D115">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4">
+      <c r="A116" t="s">
+        <v>85</v>
+      </c>
+      <c r="B116" t="s">
+        <v>22</v>
+      </c>
+      <c r="C116" t="s">
+        <v>26</v>
+      </c>
+      <c r="D116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4">
+      <c r="A117" t="s">
+        <v>137</v>
+      </c>
+      <c r="B117" t="s">
+        <v>22</v>
+      </c>
+      <c r="C117" t="s">
+        <v>26</v>
+      </c>
+      <c r="D117">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4">
+      <c r="A118" t="s">
+        <v>86</v>
+      </c>
+      <c r="B118" t="s">
+        <v>22</v>
+      </c>
+      <c r="C118" t="s">
+        <v>26</v>
+      </c>
+      <c r="D118">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4">
+      <c r="A119" t="s">
+        <v>138</v>
+      </c>
+      <c r="B119" t="s">
+        <v>22</v>
+      </c>
+      <c r="C119" t="s">
+        <v>26</v>
+      </c>
+      <c r="D119">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4">
+      <c r="A120" t="s">
+        <v>139</v>
+      </c>
+      <c r="B120" t="s">
+        <v>22</v>
+      </c>
+      <c r="C120" t="s">
+        <v>26</v>
+      </c>
+      <c r="D120">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4">
+      <c r="A121" t="s">
+        <v>140</v>
+      </c>
+      <c r="B121" t="s">
+        <v>22</v>
+      </c>
+      <c r="C121" t="s">
+        <v>26</v>
+      </c>
+      <c r="D121">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4">
+      <c r="A122" t="s">
+        <v>39</v>
+      </c>
+      <c r="B122" t="s">
+        <v>22</v>
+      </c>
+      <c r="C122" t="s">
+        <v>27</v>
+      </c>
+      <c r="D122">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4">
+      <c r="A123" t="s">
+        <v>141</v>
+      </c>
+      <c r="B123" t="s">
+        <v>22</v>
+      </c>
+      <c r="C123" t="s">
+        <v>27</v>
+      </c>
+      <c r="D123">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4">
+      <c r="A124" t="s">
+        <v>142</v>
+      </c>
+      <c r="B124" t="s">
+        <v>22</v>
+      </c>
+      <c r="C124" t="s">
+        <v>27</v>
+      </c>
+      <c r="D124">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4">
+      <c r="A125" t="s">
+        <v>143</v>
+      </c>
+      <c r="B125" t="s">
+        <v>22</v>
+      </c>
+      <c r="C125" t="s">
+        <v>27</v>
+      </c>
+      <c r="D125">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4">
+      <c r="A126" t="s">
+        <v>40</v>
+      </c>
+      <c r="B126" t="s">
+        <v>22</v>
+      </c>
+      <c r="C126" t="s">
+        <v>27</v>
+      </c>
+      <c r="D126">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4">
+      <c r="A127" t="s">
+        <v>144</v>
+      </c>
+      <c r="B127" t="s">
+        <v>22</v>
+      </c>
+      <c r="C127" t="s">
+        <v>27</v>
+      </c>
+      <c r="D127">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4">
+      <c r="A128" t="s">
+        <v>145</v>
+      </c>
+      <c r="B128" t="s">
+        <v>22</v>
+      </c>
+      <c r="C128" t="s">
+        <v>28</v>
+      </c>
+      <c r="D128">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4">
+      <c r="A129" t="s">
+        <v>146</v>
+      </c>
+      <c r="B129" t="s">
+        <v>22</v>
+      </c>
+      <c r="C129" t="s">
+        <v>28</v>
+      </c>
+      <c r="D129">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4">
+      <c r="A130" t="s">
+        <v>87</v>
+      </c>
+      <c r="B130" t="s">
+        <v>22</v>
+      </c>
+      <c r="C130" t="s">
+        <v>28</v>
+      </c>
+      <c r="D130">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4">
+      <c r="A131" t="s">
+        <v>147</v>
+      </c>
+      <c r="B131" t="s">
+        <v>22</v>
+      </c>
+      <c r="C131" t="s">
+        <v>28</v>
+      </c>
+      <c r="D131">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4">
+      <c r="A132" t="s">
+        <v>88</v>
+      </c>
+      <c r="B132" t="s">
+        <v>22</v>
+      </c>
+      <c r="C132" t="s">
+        <v>28</v>
+      </c>
+      <c r="D132">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4">
+      <c r="A133" t="s">
+        <v>148</v>
+      </c>
+      <c r="B133" t="s">
+        <v>22</v>
+      </c>
+      <c r="C133" t="s">
+        <v>28</v>
+      </c>
+      <c r="D133">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4">
+      <c r="A134" t="s">
+        <v>89</v>
+      </c>
+      <c r="B134" t="s">
+        <v>22</v>
+      </c>
+      <c r="C134" t="s">
+        <v>29</v>
+      </c>
+      <c r="D134">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4">
+      <c r="A135" t="s">
+        <v>149</v>
+      </c>
+      <c r="B135" t="s">
+        <v>22</v>
+      </c>
+      <c r="C135" t="s">
+        <v>29</v>
+      </c>
+      <c r="D135">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4">
+      <c r="A136" t="s">
+        <v>90</v>
+      </c>
+      <c r="B136" t="s">
+        <v>22</v>
+      </c>
+      <c r="C136" t="s">
+        <v>29</v>
+      </c>
+      <c r="D136">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4">
+      <c r="A137" t="s">
+        <v>150</v>
+      </c>
+      <c r="B137" t="s">
+        <v>22</v>
+      </c>
+      <c r="C137" t="s">
+        <v>29</v>
+      </c>
+      <c r="D137">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4">
+      <c r="A138" t="s">
         <v>91</v>
       </c>
-      <c r="B79" t="s">
-        <v>22</v>
-      </c>
-      <c r="C79" t="s">
+      <c r="B138" t="s">
+        <v>22</v>
+      </c>
+      <c r="C138" t="s">
         <v>29</v>
       </c>
-      <c r="D79">
+      <c r="D138">
         <v>5</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4">
+      <c r="A139" t="s">
+        <v>151</v>
+      </c>
+      <c r="B139" t="s">
+        <v>22</v>
+      </c>
+      <c r="C139" t="s">
+        <v>29</v>
+      </c>
+      <c r="D139">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>